<commit_message>
Merged results into plots_combines
</commit_message>
<xml_diff>
--- a/plots_combined.xlsx
+++ b/plots_combined.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laidlaw Research\AdaptiveNetworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{74F50ACD-FF55-4566-A5F5-B3ACEA5161A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DA6472-1572-4FC0-A54B-ED8EDE6446E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="plots_combined" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -638,6 +638,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10695815887273119"/>
+          <c:y val="2.3931623931623933E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1285,6 +1293,212 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-0635-414C-82F9-0FD6F0DFE3F6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>added_dist</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="6"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>plots_combined!$Z$4:$Z$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.04</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>plots_combined!$AE$4:$AE$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>594.38305062374604</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>539.16785329532502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>308.82087200592599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>309.01586652947299</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>273.07836454360699</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>369.18242403789202</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>162.383630890044</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.603414645028401</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.31568932821099</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>150.70982576161899</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>117.509521194743</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>120.346719536981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.985581254978101</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.709309094288102</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>26.558729321505101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.9169601148181101</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.9933900702112402</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.68404283875181</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.557018654350401</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.41941601098062</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.1437114414360501</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>11.5102429909252</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.40140358583892</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18.540703057943901</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.09365041324997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A194-45F2-9229-57DE66831A9C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2203,16 +2417,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2536,16 +2750,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AE28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2565,7 +2779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>12</v>
       </c>
@@ -2629,8 +2843,29 @@
       <c r="W4">
         <v>844.46344939999994</v>
       </c>
+      <c r="Y4">
+        <v>12</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0.5</v>
+      </c>
+      <c r="AB4">
+        <v>6</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>594.38305062374604</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>12</v>
       </c>
@@ -2694,8 +2929,29 @@
       <c r="W5">
         <v>410.2873955</v>
       </c>
+      <c r="Y5">
+        <v>12</v>
+      </c>
+      <c r="Z5">
+        <v>0.02</v>
+      </c>
+      <c r="AA5">
+        <v>0.5</v>
+      </c>
+      <c r="AB5">
+        <v>6</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>539.16785329532502</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>12</v>
       </c>
@@ -2759,8 +3015,29 @@
       <c r="W6">
         <v>140.34540509999999</v>
       </c>
+      <c r="Y6">
+        <v>12</v>
+      </c>
+      <c r="Z6">
+        <v>0.04</v>
+      </c>
+      <c r="AA6">
+        <v>0.5</v>
+      </c>
+      <c r="AB6">
+        <v>6</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>308.82087200592599</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>12</v>
       </c>
@@ -2824,8 +3101,29 @@
       <c r="W7">
         <v>51.336161769999997</v>
       </c>
+      <c r="Y7">
+        <v>12</v>
+      </c>
+      <c r="Z7">
+        <v>0.06</v>
+      </c>
+      <c r="AA7">
+        <v>0.5</v>
+      </c>
+      <c r="AB7">
+        <v>6</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <v>309.01586652947299</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>12</v>
       </c>
@@ -2889,8 +3187,29 @@
       <c r="W8">
         <v>20.937670090000001</v>
       </c>
+      <c r="Y8">
+        <v>12</v>
+      </c>
+      <c r="Z8">
+        <v>0.08</v>
+      </c>
+      <c r="AA8">
+        <v>0.5</v>
+      </c>
+      <c r="AB8">
+        <v>6</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+      <c r="AE8">
+        <v>273.07836454360699</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>12</v>
       </c>
@@ -2954,8 +3273,29 @@
       <c r="W9">
         <v>9.4436959520000006</v>
       </c>
+      <c r="Y9">
+        <v>12</v>
+      </c>
+      <c r="Z9">
+        <v>0.1</v>
+      </c>
+      <c r="AA9">
+        <v>0.5</v>
+      </c>
+      <c r="AB9">
+        <v>6</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>369.18242403789202</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>12</v>
       </c>
@@ -3019,8 +3359,29 @@
       <c r="W10">
         <v>4.7199337019999996</v>
       </c>
+      <c r="Y10">
+        <v>12</v>
+      </c>
+      <c r="Z10">
+        <v>0.12</v>
+      </c>
+      <c r="AA10">
+        <v>0.5</v>
+      </c>
+      <c r="AB10">
+        <v>6</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>162.383630890044</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>12</v>
       </c>
@@ -3084,8 +3445,29 @@
       <c r="W11">
         <v>2.983962826</v>
       </c>
+      <c r="Y11">
+        <v>12</v>
+      </c>
+      <c r="Z11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AA11">
+        <v>0.5</v>
+      </c>
+      <c r="AB11">
+        <v>6</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>40.603414645028401</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3149,8 +3531,29 @@
       <c r="W12">
         <v>2.0304601089999998</v>
       </c>
+      <c r="Y12">
+        <v>12</v>
+      </c>
+      <c r="Z12">
+        <v>0.16</v>
+      </c>
+      <c r="AA12">
+        <v>0.5</v>
+      </c>
+      <c r="AB12">
+        <v>6</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>100.31568932821099</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3214,8 +3617,29 @@
       <c r="W13">
         <v>1.477805094</v>
       </c>
+      <c r="Y13">
+        <v>12</v>
+      </c>
+      <c r="Z13">
+        <v>0.18</v>
+      </c>
+      <c r="AA13">
+        <v>0.5</v>
+      </c>
+      <c r="AB13">
+        <v>6</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>150.70982576161899</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3279,8 +3703,29 @@
       <c r="W14">
         <v>1.157143604</v>
       </c>
+      <c r="Y14">
+        <v>12</v>
+      </c>
+      <c r="Z14">
+        <v>0.2</v>
+      </c>
+      <c r="AA14">
+        <v>0.5</v>
+      </c>
+      <c r="AB14">
+        <v>6</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>117.509521194743</v>
+      </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>12</v>
       </c>
@@ -3344,8 +3789,29 @@
       <c r="W15">
         <v>0.87092879700000003</v>
       </c>
+      <c r="Y15">
+        <v>12</v>
+      </c>
+      <c r="Z15">
+        <v>0.22</v>
+      </c>
+      <c r="AA15">
+        <v>0.5</v>
+      </c>
+      <c r="AB15">
+        <v>6</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>120.346719536981</v>
+      </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -3409,8 +3875,29 @@
       <c r="W16">
         <v>0.81538187100000004</v>
       </c>
+      <c r="Y16">
+        <v>12</v>
+      </c>
+      <c r="Z16">
+        <v>0.24</v>
+      </c>
+      <c r="AA16">
+        <v>0.5</v>
+      </c>
+      <c r="AB16">
+        <v>6</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>11.985581254978101</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>12</v>
       </c>
@@ -3474,8 +3961,29 @@
       <c r="W17">
         <v>0.68847056600000001</v>
       </c>
+      <c r="Y17">
+        <v>12</v>
+      </c>
+      <c r="Z17">
+        <v>0.26</v>
+      </c>
+      <c r="AA17">
+        <v>0.5</v>
+      </c>
+      <c r="AB17">
+        <v>6</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>32.709309094288102</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>12</v>
       </c>
@@ -3539,8 +4047,29 @@
       <c r="W18">
         <v>0.60125442699999998</v>
       </c>
+      <c r="Y18">
+        <v>12</v>
+      </c>
+      <c r="Z18">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="AA18">
+        <v>0.5</v>
+      </c>
+      <c r="AB18">
+        <v>6</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>26.558729321505101</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>
@@ -3604,8 +4133,29 @@
       <c r="W19">
         <v>0.62876447899999999</v>
       </c>
+      <c r="Y19">
+        <v>12</v>
+      </c>
+      <c r="Z19">
+        <v>0.3</v>
+      </c>
+      <c r="AA19">
+        <v>0.5</v>
+      </c>
+      <c r="AB19">
+        <v>6</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>9.9169601148181101</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>12</v>
       </c>
@@ -3669,8 +4219,29 @@
       <c r="W20">
         <v>0.48974176699999999</v>
       </c>
+      <c r="Y20">
+        <v>12</v>
+      </c>
+      <c r="Z20">
+        <v>0.32</v>
+      </c>
+      <c r="AA20">
+        <v>0.5</v>
+      </c>
+      <c r="AB20">
+        <v>6</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>2.9933900702112402</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>12</v>
       </c>
@@ -3734,8 +4305,29 @@
       <c r="W21">
         <v>0.30622543899999999</v>
       </c>
+      <c r="Y21">
+        <v>12</v>
+      </c>
+      <c r="Z21">
+        <v>0.34</v>
+      </c>
+      <c r="AA21">
+        <v>0.5</v>
+      </c>
+      <c r="AB21">
+        <v>6</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>1.68404283875181</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>12</v>
       </c>
@@ -3799,8 +4391,29 @@
       <c r="W22">
         <v>0.26213070100000002</v>
       </c>
+      <c r="Y22">
+        <v>12</v>
+      </c>
+      <c r="Z22">
+        <v>0.36</v>
+      </c>
+      <c r="AA22">
+        <v>0.5</v>
+      </c>
+      <c r="AB22">
+        <v>6</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>19.557018654350401</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>12</v>
       </c>
@@ -3864,8 +4477,29 @@
       <c r="W23">
         <v>0.22015135199999999</v>
       </c>
+      <c r="Y23">
+        <v>12</v>
+      </c>
+      <c r="Z23">
+        <v>0.38</v>
+      </c>
+      <c r="AA23">
+        <v>0.5</v>
+      </c>
+      <c r="AB23">
+        <v>6</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>2.41941601098062</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>12</v>
       </c>
@@ -3929,8 +4563,29 @@
       <c r="W24">
         <v>0.29189713299999998</v>
       </c>
+      <c r="Y24">
+        <v>12</v>
+      </c>
+      <c r="Z24">
+        <v>0.4</v>
+      </c>
+      <c r="AA24">
+        <v>0.5</v>
+      </c>
+      <c r="AB24">
+        <v>6</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>2.1437114414360501</v>
+      </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
@@ -3994,8 +4649,29 @@
       <c r="W25">
         <v>0.22052169799999999</v>
       </c>
+      <c r="Y25">
+        <v>12</v>
+      </c>
+      <c r="Z25">
+        <v>0.42</v>
+      </c>
+      <c r="AA25">
+        <v>0.5</v>
+      </c>
+      <c r="AB25">
+        <v>6</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>11.5102429909252</v>
+      </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>12</v>
       </c>
@@ -4059,8 +4735,29 @@
       <c r="W26">
         <v>0.25221619099999998</v>
       </c>
+      <c r="Y26">
+        <v>12</v>
+      </c>
+      <c r="Z26">
+        <v>0.44</v>
+      </c>
+      <c r="AA26">
+        <v>0.5</v>
+      </c>
+      <c r="AB26">
+        <v>6</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>0</v>
+      </c>
+      <c r="AE26">
+        <v>1.40140358583892</v>
+      </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>12</v>
       </c>
@@ -4124,8 +4821,29 @@
       <c r="W27">
         <v>0.226113394</v>
       </c>
+      <c r="Y27">
+        <v>12</v>
+      </c>
+      <c r="Z27">
+        <v>0.46</v>
+      </c>
+      <c r="AA27">
+        <v>0.5</v>
+      </c>
+      <c r="AB27">
+        <v>6</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0</v>
+      </c>
+      <c r="AE27">
+        <v>18.540703057943901</v>
+      </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>12</v>
       </c>
@@ -4188,6 +4906,27 @@
       </c>
       <c r="W28">
         <v>0.17552567999999999</v>
+      </c>
+      <c r="Y28">
+        <v>12</v>
+      </c>
+      <c r="Z28">
+        <v>0.48</v>
+      </c>
+      <c r="AA28">
+        <v>0.5</v>
+      </c>
+      <c r="AB28">
+        <v>6</v>
+      </c>
+      <c r="AC28">
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <v>0</v>
+      </c>
+      <c r="AE28">
+        <v>3.09365041324997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>